<commit_message>
BOM updated to Rev 0.4
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -15,7 +15,7 @@
     <sheet name="SAMPad" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SAMPad!$A$1:$F$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SAMPad!$A$1:$F$26</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Table4[#All]</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="123">
   <si>
     <t>Value</t>
   </si>
@@ -214,57 +214,12 @@
     <t>Panasonic</t>
   </si>
   <si>
-    <t>C15</t>
-  </si>
-  <si>
-    <t>4.7uF</t>
-  </si>
-  <si>
-    <t>CAP CER 4.7UF 6.3V X5R 0805</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>AP3417C</t>
-  </si>
-  <si>
-    <t>IC REG BUCK ADJ 1A SYNC SOT25</t>
-  </si>
-  <si>
-    <t>AP3417CKTR-G1</t>
-  </si>
-  <si>
     <t>Diodes Inc</t>
   </si>
   <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>2.2uH</t>
-  </si>
-  <si>
-    <t>FIXED IND 2.2UH 2.9A 44 MOHM SMD</t>
-  </si>
-  <si>
-    <t>SRN4018-2R2M</t>
-  </si>
-  <si>
     <t>Bourns Inc</t>
   </si>
   <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>453k</t>
-  </si>
-  <si>
-    <t>RES SMD 453K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>RC0805FR-07453KL</t>
-  </si>
-  <si>
     <t>Yageo</t>
   </si>
   <si>
@@ -346,15 +301,9 @@
     <t>RI1 - RI7</t>
   </si>
   <si>
-    <t>R8, R9, R14</t>
-  </si>
-  <si>
     <t>R34, R35</t>
   </si>
   <si>
-    <t>C9, C16 - C18</t>
-  </si>
-  <si>
     <t>C13, C14</t>
   </si>
   <si>
@@ -391,9 +340,6 @@
     <t>CC0805KKX7R6BB105</t>
   </si>
   <si>
-    <t>CC0805MKX5R5BB475</t>
-  </si>
-  <si>
     <t>CC0805DRNPO9BN8R0</t>
   </si>
   <si>
@@ -440,6 +386,12 @@
   </si>
   <si>
     <t>Buzzer (Optional)</t>
+  </si>
+  <si>
+    <t>R9, R14</t>
+  </si>
+  <si>
+    <t>C9, C17 - C18</t>
   </si>
 </sst>
 </file>
@@ -1044,8 +996,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:F39" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:F39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:F35" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:F35"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Ref"/>
     <tableColumn id="2" name="Value"/>
@@ -1324,10 +1276,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F39"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,13 +1294,13 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1362,7 +1314,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
@@ -1374,15 +1326,15 @@
         <v>31</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
         <v>49</v>
@@ -1394,645 +1346,565 @@
         <v>50</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6">
         <v>1</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6">
-        <v>9</v>
-      </c>
       <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>80</v>
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" t="s">
-        <v>62</v>
+        <v>24</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>37</v>
       </c>
       <c r="C8">
-        <v>24</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>70</v>
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" t="s">
-        <v>40</v>
+      <c r="D9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>75</v>
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>75</v>
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14" t="s">
-        <v>22</v>
+      <c r="D14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>330</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" t="s">
-        <v>46</v>
+        <v>13</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16">
+        <v>73</v>
+      </c>
+      <c r="C16" s="4">
         <v>1</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>120</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>90</v>
       </c>
       <c r="B17">
-        <v>330</v>
+        <v>22</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>87</v>
-      </c>
-      <c r="B18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" s="4">
+        <v>56</v>
+      </c>
+      <c r="B18">
+        <v>100</v>
+      </c>
+      <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E18" s="4"/>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="F18" s="4" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>105</v>
-      </c>
-      <c r="B19">
-        <v>22</v>
+        <v>121</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="B20">
-        <v>100</v>
+        <v>470</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>114</v>
+        <v>20</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>80</v>
+      <c r="D21" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>80</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>106</v>
-      </c>
-      <c r="B23">
-        <v>470</v>
+        <v>85</v>
+      </c>
+      <c r="B23" t="s">
+        <v>86</v>
       </c>
       <c r="C23">
-        <v>7</v>
-      </c>
-      <c r="D23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>80</v>
+        <v>1</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F23" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>130</v>
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
       </c>
       <c r="F24" t="s">
-        <v>132</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="C25">
-        <v>24</v>
-      </c>
-      <c r="D25" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>128</v>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
+        <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>70</v>
+      <c r="A28" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>70</v>
+      <c r="D29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="B30" t="s">
-        <v>124</v>
+        <v>79</v>
       </c>
       <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>137</v>
-      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>90</v>
-      </c>
-      <c r="B33" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>92</v>
-      </c>
-      <c r="E33" t="s">
-        <v>93</v>
-      </c>
-      <c r="F33" t="s">
-        <v>75</v>
+      <c r="A33" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>52</v>
       </c>
       <c r="C34">
-        <v>2</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>80</v>
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>133</v>
+      <c r="A35" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C35">
-        <v>2</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>121</v>
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D36" s="4"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38" t="s">
-        <v>53</v>
-      </c>
-      <c r="E38" t="s">
-        <v>54</v>
-      </c>
-      <c r="F38" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B39" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>